<commit_message>
Updated Bulk Upload with actions
</commit_message>
<xml_diff>
--- a/flask_API/empData.xlsx
+++ b/flask_API/empData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fbd1fb2900fa257/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{55602F56-A45A-46C9-A8F1-49F25EE7D87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="14_{55602F56-A45A-46C9-A8F1-49F25EE7D87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A4DA0F-DAD3-49D7-BA00-2CA67422EBA4}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4A58C7B9-8E0B-48CF-B2B8-6CD00F8DD483}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11235" xr2:uid="{4A58C7B9-8E0B-48CF-B2B8-6CD00F8DD483}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
   <si>
     <t>empId</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Bhaskar</t>
   </si>
   <si>
-    <t>Annapurna</t>
-  </si>
-  <si>
     <t>Dishan</t>
   </si>
   <si>
@@ -255,6 +252,30 @@
   </si>
   <si>
     <t>Full Stack Engineer</t>
+  </si>
+  <si>
+    <t>Dhanush</t>
+  </si>
+  <si>
+    <t>emp033</t>
+  </si>
+  <si>
+    <t>Koushik</t>
+  </si>
+  <si>
+    <t>Intern</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Delete</t>
   </si>
 </sst>
 </file>
@@ -313,6 +334,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -612,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC64E2C4-DD6A-49EB-B31D-BE32250B5B14}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +651,7 @@
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,8 +664,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -648,14 +676,17 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D6" si="0">_xlfn.CONCAT(A2,"@emp.com")</f>
         <v>emp001@emp.com</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -663,14 +694,17 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
         <v>emp002@emp.com</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -678,49 +712,58 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
         <v>emp003@emp.com</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>emp004@emp.com</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>emp005@emp.com</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -729,73 +772,88 @@
         <f>_xlfn.CONCAT(A7,"@emp.com")</f>
         <v>emp006@emp.com</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" ref="D8:D33" si="1">_xlfn.CONCAT(A8,"@emp.com")</f>
+        <f t="shared" ref="D8:D34" si="1">_xlfn.CONCAT(A8,"@emp.com")</f>
         <v>emp007@emp.com</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="1"/>
         <v>emp008@emp.com</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="1"/>
         <v>emp009@emp.com</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="1"/>
         <v>emp010@emp.com</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -804,73 +862,88 @@
         <f t="shared" si="1"/>
         <v>emp011@emp.com</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
         <v>emp012@emp.com</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="1"/>
         <v>emp013@emp.com</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="1"/>
         <v>emp014@emp.com</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="1"/>
         <v>emp015@emp.com</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -879,73 +952,88 @@
         <f t="shared" si="1"/>
         <v>emp016@emp.com</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="1"/>
         <v>emp017@emp.com</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="1"/>
         <v>emp018@emp.com</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="1"/>
         <v>emp019@emp.com</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="1"/>
         <v>emp020@emp.com</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -954,73 +1042,88 @@
         <f t="shared" si="1"/>
         <v>emp021@emp.com</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="1"/>
         <v>emp022@emp.com</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="1"/>
         <v>emp023@emp.com</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="1"/>
         <v>emp024@emp.com</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="1"/>
         <v>emp025@emp.com</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -1029,73 +1132,88 @@
         <f t="shared" si="1"/>
         <v>emp026@emp.com</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="1"/>
         <v>emp027@emp.com</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="1"/>
         <v>emp028@emp.com</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="1"/>
         <v>emp029@emp.com</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="1"/>
         <v>emp030@emp.com</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1104,20 +1222,44 @@
         <f t="shared" si="1"/>
         <v>emp031@emp.com</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
       <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
       <c r="D33" t="str">
         <f t="shared" si="1"/>
         <v>emp032@emp.com</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>emp033@emp.com</v>
+      </c>
+      <c r="E34" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>